<commit_message>
modified diff driver paramter
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08079635-7652-4EAE-A021-689B8D600641}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="2790" windowWidth="18000" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="2790" windowWidth="18000" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -133,13 +132,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.000000000000000_ "/>
     <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="178" formatCode="0.0000000000_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -278,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -310,27 +309,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,24 +343,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -555,14 +518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="14.75" customWidth="1"/>
@@ -570,14 +533,14 @@
     <col min="5" max="5" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -585,10 +548,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -596,10 +559,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -610,7 +573,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="14.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -619,10 +582,10 @@
       </c>
       <c r="C5" s="3">
         <f>3.1415926*C2/C3</f>
-        <v>0.10154642747474747</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>0.16689710687500001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -631,10 +594,10 @@
       </c>
       <c r="C6" s="3">
         <f>3.1415926*C2/C3/1000</f>
-        <v>1.0154642747474747E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1.66897106875E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -643,10 +606,10 @@
       </c>
       <c r="C7" s="4">
         <f>C3/(3.1415926*C2/1000)</f>
-        <v>9847.7122717948841</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>5991.7156068437089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -655,10 +618,10 @@
       </c>
       <c r="C8" s="5">
         <f>C3/(3.1415926*C2)</f>
-        <v>9.8477122717948848</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>5.9917156068437087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -667,10 +630,10 @@
       </c>
       <c r="C9" s="6">
         <f>3.1415926/C3*2</f>
-        <v>3.1733258585858585E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>1.9634953750000002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -679,10 +642,10 @@
       </c>
       <c r="C10" s="6">
         <f>360/C3</f>
-        <v>0.18181818181818182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -693,7 +656,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="14.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -702,10 +665,10 @@
       </c>
       <c r="C12">
         <f>(3.1415926*C2*C11/60)</f>
-        <v>1172.8612373333335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>3115.4126616666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -716,7 +679,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="14.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -727,7 +690,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="14.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -736,7 +699,7 @@
       </c>
       <c r="C15">
         <f>(C14*10000*C3*C13/31415926/C2)</f>
-        <v>59.086273630769313</v>
+        <v>35.950293641062252</v>
       </c>
     </row>
   </sheetData>
@@ -750,12 +713,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -764,12 +727,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>